<commit_message>
Cap nhat nhat ky
</commit_message>
<xml_diff>
--- a/report/Nhom57_NguyenTienDat_VoTrungHieu_KeHoach&ThucHien.xlsx
+++ b/report/Nhom57_NguyenTienDat_VoTrungHieu_KeHoach&ThucHien.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KhoaLuan\KLTN_Tour\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thang\OneDrive\Máy tính\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08365633-F217-4C03-9ED6-80DE65D22D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D451025A-0BE9-462A-BD31-0ED1B34C3651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nhom57_ThucHien" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t>NHẬT KÝ LÀM VIỆC</t>
   </si>
@@ -224,25 +224,8 @@
 - Chỉnh sửa tài liệu báo cáo, hệ thống hoá nghiệp vụ một cách chi tiết.</t>
   </si>
   <si>
-    <t>- Update Use case tổng quát và đặc tả Use case
-- Hiện thực ứng dụng</t>
-  </si>
-  <si>
-    <t>- Fix một số bug sau khi kiểm thử
-- Tiếp tục kiểm thử chức năng
-- Tiếp tục hoàn thiện code phần Admin</t>
-  </si>
-  <si>
     <t>- Chỉnh sửa tài liệu
 - Bổ sung các công nghệ sử dụng trong đề tài, soạn slide báo cáo</t>
-  </si>
-  <si>
-    <t>- Đặc tả Use case
-- Hiện thực ứng dụng (50%): Xác thực người dùng, Trang chủ, Thông tin hồ sơ cá nhân, Quản lý Tour, Đăng ký, Đăng nhập.</t>
-  </si>
-  <si>
-    <t>- Đặc tả Use case 
-- Hiện thực ứng dụng (70%): Xác thực người dùng, Trang chủ, Thông tin hồ sơ cá nhân, Quản lý Tour, Đăng ký, Đăng nhập, Đặt tour, Xem thông tin vé đã đặt.</t>
   </si>
   <si>
     <t>- Kiểm thử tích hợp
@@ -309,11 +292,6 @@
 - Hiện thực web (90%): Quản lý thông tin tài khoản, chức năng thống kê cho từng tour.</t>
   </si>
   <si>
-    <t>- Hoàn thiện  App.
-- Hoàn thiện website
-- Kiểm thử các chức năng đã hoàn thiện</t>
-  </si>
-  <si>
     <t xml:space="preserve">- Deploy và chuyển đổi các API.
 - Deploy web với service Hosting (firebase) </t>
   </si>
@@ -324,6 +302,42 @@
   </si>
   <si>
     <t>Hoàn thiện tài liệu, slide báo cáo, file nhật ký</t>
+  </si>
+  <si>
+    <t>Chuẩn bị đầy đủ tài liệu, cần chỉnh sửa lại các mục của tài liệu cho phù hợp</t>
+  </si>
+  <si>
+    <t>Thêm video vào trong chuyến đi để có thêm nhiều lựa chọn cho khách hàng.</t>
+  </si>
+  <si>
+    <t>- Cập nhật file kế hoạch thực tế</t>
+  </si>
+  <si>
+    <t>- Hoàn thiện  App.
+- Hoàn thiện website</t>
+  </si>
+  <si>
+    <t>- Kiểm thử chức năng 
+- Fix một số bug sau khi kiểm thử</t>
+  </si>
+  <si>
+    <t>Có thể thêm chức năng đặt tour để đa dạng.</t>
+  </si>
+  <si>
+    <t>Còn cần tiếp tục hoàn thiện</t>
+  </si>
+  <si>
+    <t>- Đặc tả Use case
+- Viết API cho các chức năng (40%)
+- Hiện thực ứng dụng (50%): Xác thực người dùng, Trang chủ, Thông tin hồ sơ cá nhân, Quản lý Tour, Đăng ký, Đăng nhập
+- Hiện thực website (40%): Trang đăng nhập, trang chủ.</t>
+  </si>
+  <si>
+    <t>- Tiếp tục kiểm thử chức năng
+- Fix một số bug sau khi kiểm thử</t>
+  </si>
+  <si>
+    <t>Thêm 1 tùy chọn khoảng cách(100km) trong chuyến đi để dễ dàng kiểm tra và thống kê cần phải chi tiết hơn</t>
   </si>
 </sst>
 </file>
@@ -837,10 +851,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1162,22 +1176,22 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="19.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="3" customWidth="1"/>
-    <col min="2" max="2" width="24.375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="25.375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="18.125" style="70" customWidth="1"/>
-    <col min="5" max="5" width="64.875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="32.75" style="3" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" style="70" customWidth="1"/>
+    <col min="5" max="5" width="64.88671875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="32.77734375" style="3" customWidth="1"/>
     <col min="7" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="49.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="49.35" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1188,7 +1202,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1201,7 +1215,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1213,7 +1227,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1225,7 +1239,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:9" ht="23.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -1238,7 +1252,7 @@
       <c r="F5" s="5"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -1251,7 +1265,7 @@
       <c r="F6" s="25"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:9" s="13" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="13" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="52" t="s">
         <v>6</v>
       </c>
@@ -1272,7 +1286,7 @@
       </c>
       <c r="G7" s="12"/>
     </row>
-    <row r="8" spans="1:9" s="29" customFormat="1" ht="39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="29" customFormat="1" ht="38.4" x14ac:dyDescent="0.3">
       <c r="A8" s="41">
         <v>1</v>
       </c>
@@ -1291,7 +1305,7 @@
       <c r="F8" s="56"/>
       <c r="I8" s="34"/>
     </row>
-    <row r="9" spans="1:9" s="29" customFormat="1" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="29" customFormat="1" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="57">
         <v>2</v>
       </c>
@@ -1308,7 +1322,7 @@
       </c>
       <c r="F9" s="56"/>
     </row>
-    <row r="10" spans="1:9" s="29" customFormat="1" ht="120.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="29" customFormat="1" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="57">
         <v>4</v>
       </c>
@@ -1324,17 +1338,19 @@
         <v>44930</v>
       </c>
       <c r="E10" s="56" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="56"/>
+        <v>29</v>
+      </c>
+      <c r="F10" s="56" t="s">
+        <v>39</v>
+      </c>
       <c r="I10" s="34"/>
     </row>
-    <row r="11" spans="1:9" s="29" customFormat="1" ht="270" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="29" customFormat="1" ht="282.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="57">
         <v>5</v>
       </c>
       <c r="B11" s="59">
-        <f t="shared" ref="B11:B22" si="0">C10+1</f>
+        <f>C10+1</f>
         <v>44935</v>
       </c>
       <c r="C11" s="61">
@@ -1343,16 +1359,16 @@
       </c>
       <c r="D11" s="66"/>
       <c r="E11" s="56" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="72"/>
-    </row>
-    <row r="12" spans="1:9" s="29" customFormat="1" ht="156" customHeight="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="F11" s="56"/>
+    </row>
+    <row r="12" spans="1:9" s="29" customFormat="1" ht="144.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="57">
         <v>6</v>
       </c>
       <c r="B12" s="59">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B12:B22" si="0">C11+1</f>
         <v>44942</v>
       </c>
       <c r="C12" s="59">
@@ -1361,12 +1377,12 @@
       </c>
       <c r="D12" s="66"/>
       <c r="E12" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="73"/>
+        <v>32</v>
+      </c>
+      <c r="F12" s="56"/>
       <c r="I12" s="34"/>
     </row>
-    <row r="13" spans="1:9" s="29" customFormat="1" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="29" customFormat="1" ht="135.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="57">
         <v>7</v>
       </c>
@@ -1382,11 +1398,13 @@
         <v>44964</v>
       </c>
       <c r="E13" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="56"/>
-    </row>
-    <row r="14" spans="1:9" s="29" customFormat="1" ht="136.5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="F13" s="56" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="29" customFormat="1" ht="153.6" x14ac:dyDescent="0.3">
       <c r="A14" s="57">
         <v>8</v>
       </c>
@@ -1400,12 +1418,12 @@
       </c>
       <c r="D14" s="66"/>
       <c r="E14" s="62" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F14" s="56"/>
       <c r="I14" s="34"/>
     </row>
-    <row r="15" spans="1:9" s="29" customFormat="1" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="29" customFormat="1" ht="153" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="57">
         <v>9</v>
       </c>
@@ -1419,11 +1437,11 @@
       </c>
       <c r="D15" s="66"/>
       <c r="E15" s="56" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F15" s="56"/>
     </row>
-    <row r="16" spans="1:9" s="29" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="29" customFormat="1" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="57">
         <v>10</v>
       </c>
@@ -1439,12 +1457,14 @@
         <v>44987</v>
       </c>
       <c r="E16" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="56"/>
+        <v>42</v>
+      </c>
+      <c r="F16" s="56" t="s">
+        <v>45</v>
+      </c>
       <c r="I16" s="34"/>
     </row>
-    <row r="17" spans="1:9" s="29" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="29" customFormat="1" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="57">
         <v>11</v>
       </c>
@@ -1458,11 +1478,11 @@
       </c>
       <c r="D17" s="66"/>
       <c r="E17" s="56" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="F17" s="56"/>
     </row>
-    <row r="18" spans="1:9" s="29" customFormat="1" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="29" customFormat="1" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="57">
         <v>12</v>
       </c>
@@ -1476,11 +1496,11 @@
       </c>
       <c r="D18" s="66"/>
       <c r="E18" s="56" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F18" s="56"/>
     </row>
-    <row r="19" spans="1:9" s="29" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="29" customFormat="1" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="57">
         <v>13</v>
       </c>
@@ -1496,12 +1516,14 @@
         <v>45008</v>
       </c>
       <c r="E19" s="56" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="56"/>
+        <v>36</v>
+      </c>
+      <c r="F19" s="56" t="s">
+        <v>40</v>
+      </c>
       <c r="I19" s="34"/>
     </row>
-    <row r="20" spans="1:9" s="29" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="29" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="57">
         <v>14</v>
       </c>
@@ -1514,11 +1536,11 @@
         <v>45018</v>
       </c>
       <c r="E20" s="56" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="F20" s="56"/>
     </row>
-    <row r="21" spans="1:9" s="29" customFormat="1" ht="78" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="29" customFormat="1" ht="96" x14ac:dyDescent="0.3">
       <c r="A21" s="57">
         <v>15</v>
       </c>
@@ -1534,12 +1556,14 @@
         <v>45020</v>
       </c>
       <c r="E21" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="F21" s="56"/>
+        <v>37</v>
+      </c>
+      <c r="F21" s="56" t="s">
+        <v>48</v>
+      </c>
       <c r="I21" s="34"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="57">
         <v>16</v>
       </c>
@@ -1553,16 +1577,61 @@
       </c>
       <c r="D22" s="55"/>
       <c r="E22" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="55"/>
-    </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F22" s="56"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F23" s="72"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F24" s="73"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F25" s="28"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F26" s="28"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F27" s="28"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F28" s="28"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F29" s="28"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F30" s="28"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F31" s="28"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F32" s="28"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F33" s="28"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F34" s="29"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F35" s="29"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F36" s="29"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F37" s="29"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D98" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F23:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1574,22 +1643,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="G20" sqref="G9:G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="3" customWidth="1"/>
-    <col min="2" max="2" width="24.375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="25.375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="64.875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="64.88671875" style="3" customWidth="1"/>
     <col min="5" max="5" width="9" style="29" customWidth="1"/>
     <col min="6" max="6" width="9" style="3" customWidth="1"/>
     <col min="7" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="49.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="49.35" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1599,7 +1668,7 @@
       <c r="E1" s="23"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1611,7 +1680,7 @@
       <c r="E2" s="24"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1622,7 +1691,7 @@
       <c r="D3" s="5"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1633,7 +1702,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -1645,7 +1714,7 @@
       <c r="E5" s="24"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -1657,7 +1726,7 @@
       <c r="E6" s="25"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:8" s="13" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="13" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="35" t="s">
         <v>6</v>
       </c>
@@ -1673,7 +1742,7 @@
       <c r="E7" s="26"/>
       <c r="F7" s="12"/>
     </row>
-    <row r="8" spans="1:8" s="42" customFormat="1" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="42" customFormat="1" ht="54.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="41">
         <v>1</v>
       </c>
@@ -1689,7 +1758,7 @@
       <c r="E8" s="44"/>
       <c r="F8" s="45"/>
     </row>
-    <row r="9" spans="1:8" ht="97.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="96" x14ac:dyDescent="0.3">
       <c r="A9" s="38">
         <v>2</v>
       </c>
@@ -1707,7 +1776,7 @@
       <c r="E9" s="27"/>
       <c r="F9" s="15"/>
     </row>
-    <row r="10" spans="1:8" ht="117" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>4</v>
       </c>
@@ -1725,7 +1794,7 @@
       <c r="E10" s="28"/>
       <c r="H10" s="16"/>
     </row>
-    <row r="11" spans="1:8" ht="254.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="254.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14">
         <v>5</v>
       </c>
@@ -1742,7 +1811,7 @@
       </c>
       <c r="E11" s="28"/>
     </row>
-    <row r="12" spans="1:8" ht="151.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14">
         <v>6</v>
       </c>
@@ -1755,12 +1824,12 @@
         <v>44948</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E12" s="28"/>
       <c r="H12" s="16"/>
     </row>
-    <row r="13" spans="1:8" ht="130.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="136.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
         <v>7</v>
       </c>
@@ -1773,11 +1842,11 @@
         <v>44969</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E13" s="50"/>
     </row>
-    <row r="14" spans="1:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="153.6" x14ac:dyDescent="0.3">
       <c r="A14" s="14">
         <v>8</v>
       </c>
@@ -1790,12 +1859,12 @@
         <v>44976</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E14" s="51"/>
       <c r="H14" s="16"/>
     </row>
-    <row r="15" spans="1:8" s="49" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="49" customFormat="1" ht="172.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14">
         <v>9</v>
       </c>
@@ -1808,11 +1877,11 @@
         <v>44983</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E15" s="48"/>
     </row>
-    <row r="16" spans="1:8" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14">
         <v>10</v>
       </c>
@@ -1825,12 +1894,12 @@
         <v>44990</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E16" s="28"/>
       <c r="H16" s="16"/>
     </row>
-    <row r="17" spans="1:8" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14">
         <v>11</v>
       </c>
@@ -1843,11 +1912,11 @@
         <v>44997</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="E17" s="28"/>
     </row>
-    <row r="18" spans="1:8" ht="127.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14">
         <v>12</v>
       </c>
@@ -1860,12 +1929,12 @@
         <v>45004</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E18" s="28"/>
       <c r="H18" s="16"/>
     </row>
-    <row r="19" spans="1:8" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14">
         <v>13</v>
       </c>
@@ -1882,7 +1951,7 @@
       </c>
       <c r="E19" s="28"/>
     </row>
-    <row r="20" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14">
         <v>14</v>
       </c>
@@ -1895,12 +1964,12 @@
         <v>45018</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E20" s="28"/>
       <c r="H20" s="16"/>
     </row>
-    <row r="21" spans="1:8" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14">
         <v>15</v>
       </c>

</xml_diff>